<commit_message>
Pete: 5/29 @ 1942
</commit_message>
<xml_diff>
--- a/df.sum.xlsx
+++ b/df.sum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steamboat II\Documents\R\578project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF06D898-B12E-494D-9640-ED3312C80AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE876F28-5BC9-41B5-A460-C3195E0204B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="1275" windowWidth="28800" windowHeight="12090" xr2:uid="{C0559229-79EF-4EEA-8B4C-99A31EC2FA22}"/>
+    <workbookView xWindow="3735" yWindow="2130" windowWidth="28800" windowHeight="12090" xr2:uid="{C0559229-79EF-4EEA-8B4C-99A31EC2FA22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,19 +131,19 @@
     <t>Age Group</t>
   </si>
   <si>
-    <t>Age.Strata</t>
-  </si>
-  <si>
-    <t>0 denotes 49 or younger. 1 denotes 50 or older. 2 denotes 65 or older.</t>
-  </si>
-  <si>
     <t>Wall Motion Strata</t>
   </si>
   <si>
-    <t>WMI.S</t>
-  </si>
-  <si>
-    <t>Binary Variable. 0 denotes that WMI is less than or equal to 1.28. 1 denotes that WMI is greater than or equal to 1.28.</t>
+    <t>Age.S</t>
+  </si>
+  <si>
+    <t>WMS.S</t>
+  </si>
+  <si>
+    <t>0 denotes younger than 55 years . 1 denotes 55 - 70 years. 2 denotes older than 70</t>
+  </si>
+  <si>
+    <t>0 denotes score less than 11, 1 denotes score 12-14, 2 denotes score greater than 14</t>
   </si>
 </sst>
 </file>
@@ -563,10 +563,10 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,10 +637,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>

</xml_diff>